<commit_message>
fix #53 support format double
</commit_message>
<xml_diff>
--- a/transfer/src/test/resources/data.xlsx
+++ b/transfer/src/test/resources/data.xlsx
@@ -1,28 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaostone/workspace/beangle/data/transfer/src/test/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="460" windowWidth="49720" windowHeight="28340" tabRatio="500"/>
+    <workbookView windowWidth="19200" windowHeight="7280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -39,7 +26,6 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">name
@@ -53,10 +39,9 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>birthday:Date</t>
+          <t>idcard:String</t>
         </r>
       </text>
     </comment>
@@ -66,10 +51,9 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>birthAt:Time</t>
+          <t>birthday:Date</t>
         </r>
       </text>
     </comment>
@@ -79,34 +63,43 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>birthAt:Time</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
           <t>income:Double</t>
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="1">
+    <comment ref="F1" authorId="1">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="ＭＳ Ｐゴシック"/>
+            <rFont val="MS PGothic"/>
             <charset val="128"/>
           </rPr>
           <t>graduateOn:YearMonth</t>
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>updatedAt:DateTime</t>
@@ -118,15 +111,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>姓名</t>
+  </si>
+  <si>
+    <t>身份证号</t>
   </si>
   <si>
     <t>出生日期</t>
   </si>
   <si>
+    <t>出生时间</t>
+  </si>
+  <si>
     <t>年收入</t>
+  </si>
+  <si>
+    <t>毕业年月</t>
   </si>
   <si>
     <t>更新日期</t>
@@ -134,32 +136,23 @@
   <si>
     <t>Jack</t>
   </si>
-  <si>
-    <t>出生时间</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>毕业年月</t>
-    <rPh sb="0" eb="1">
-      <t>bi y</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>nian yue</t>
-    </rPh>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="0.000_ "/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="9">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="yyyy/m/d\ h:mm:ss"/>
     <numFmt numFmtId="177" formatCode="h:mm:ss;@"/>
-    <numFmt numFmtId="179" formatCode="yyyy/m/d\ h:mm:ss"/>
-    <numFmt numFmtId="182" formatCode="yyyy&quot;年&quot;m&quot;月&quot;;@"/>
+    <numFmt numFmtId="178" formatCode="0_ "/>
+    <numFmt numFmtId="179" formatCode="0.000_ "/>
+    <numFmt numFmtId="180" formatCode="yyyy&quot;年&quot;m&quot;月&quot;;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="25">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -168,40 +161,371 @@
     <font>
       <sz val="10"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="81"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <charset val="128"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Abadi MT Condensed Extra Bold"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="MS PGothic"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -209,24 +533,314 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -488,24 +1102,25 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.5" outlineLevelRow="1" outlineLevelCol="6"/>
   <cols>
-    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.0909090909091" customWidth="1"/>
+    <col min="7" max="7" width="23.3363636363636" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" ht="13" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -513,46 +1128,51 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="7" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="5">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1234567890111</v>
+      </c>
+      <c r="C2" s="4">
         <v>36800</v>
       </c>
-      <c r="C2" s="2">
-        <v>0.31579861111111102</v>
-      </c>
-      <c r="D2" s="3">
+      <c r="D2" s="5">
+        <v>0.315798611111111</v>
+      </c>
+      <c r="E2" s="6">
         <v>123.456</v>
       </c>
-      <c r="E2" s="6">
+      <c r="F2" s="7">
         <v>36342</v>
       </c>
-      <c r="F2" s="4">
-        <v>43821.437893518501</v>
+      <c r="G2" s="8">
+        <v>43821.4378935185</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>